<commit_message>
20161104 order-web change backP
</commit_message>
<xml_diff>
--- a/ui/享运需求进度20161102.xlsx
+++ b/ui/享运需求进度20161102.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>app端需求：</t>
   </si>
@@ -183,6 +183,10 @@
   </si>
   <si>
     <t>需要一个录入司机、电话、车辆信息 车型，路线，备注的入口和目前已在平台注册的司机做个筛选 筛出未注册司机</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>完</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -662,7 +666,7 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -853,8 +857,8 @@
       <c r="A24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="13">
-        <v>0.5</v>
+      <c r="B24" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18.75">

</xml_diff>